<commit_message>
inserindo casos de uso
</commit_message>
<xml_diff>
--- a/TCC/APS/CasosUso/CasoUsoGeral.xlsx
+++ b/TCC/APS/CasosUso/CasoUsoGeral.xlsx
@@ -584,39 +584,6 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -629,6 +596,39 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -912,29 +912,29 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:C138"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A123" workbookViewId="0">
-      <selection activeCell="B136" sqref="B136"/>
+    <sheetView tabSelected="1" topLeftCell="A138" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4:C138"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="6"/>
-    <col min="2" max="2" width="42.140625" style="9" customWidth="1"/>
-    <col min="3" max="3" width="104.85546875" style="6" customWidth="1"/>
+    <col min="2" max="2" width="31.140625" style="9" customWidth="1"/>
+    <col min="3" max="3" width="61.85546875" style="6" customWidth="1"/>
     <col min="4" max="16384" width="9.140625" style="6"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:3" ht="15" x14ac:dyDescent="0.2">
-      <c r="B1" s="32"/>
-      <c r="C1" s="32"/>
+      <c r="B1" s="37"/>
+      <c r="C1" s="37"/>
     </row>
     <row r="2" spans="2:3" ht="15" x14ac:dyDescent="0.2">
-      <c r="B2" s="32"/>
-      <c r="C2" s="32"/>
+      <c r="B2" s="37"/>
+      <c r="C2" s="37"/>
     </row>
     <row r="3" spans="2:3" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="32"/>
-      <c r="C3" s="32"/>
+      <c r="B3" s="37"/>
+      <c r="C3" s="37"/>
     </row>
     <row r="4" spans="2:3" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B4" s="11" t="s">
@@ -960,7 +960,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="2:3" s="13" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:3" s="13" customFormat="1" ht="30.75" x14ac:dyDescent="0.25">
       <c r="B7" s="11" t="s">
         <v>3</v>
       </c>
@@ -998,7 +998,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="12" spans="2:3" s="13" customFormat="1" ht="30" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:3" s="13" customFormat="1" ht="45" x14ac:dyDescent="0.2">
       <c r="B12" s="25" t="s">
         <v>10</v>
       </c>
@@ -1007,7 +1007,7 @@
       </c>
     </row>
     <row r="13" spans="2:3" ht="15" x14ac:dyDescent="0.2">
-      <c r="B13" s="33" t="s">
+      <c r="B13" s="38" t="s">
         <v>12</v>
       </c>
       <c r="C13" s="2" t="s">
@@ -1015,13 +1015,13 @@
       </c>
     </row>
     <row r="14" spans="2:3" ht="15" x14ac:dyDescent="0.2">
-      <c r="B14" s="33"/>
+      <c r="B14" s="38"/>
       <c r="C14" s="2" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="15" spans="2:3" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="34"/>
+      <c r="B15" s="39"/>
       <c r="C15" s="3" t="s">
         <v>15</v>
       </c>
@@ -1050,7 +1050,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="20" spans="2:3" ht="30" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:3" ht="45" x14ac:dyDescent="0.2">
       <c r="B20" s="14" t="s">
         <v>3</v>
       </c>
@@ -1066,7 +1066,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="22" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:3" ht="30" x14ac:dyDescent="0.2">
       <c r="B22" s="14" t="s">
         <v>6</v>
       </c>
@@ -1088,7 +1088,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="25" spans="2:3" ht="60" x14ac:dyDescent="0.2">
+    <row r="25" spans="2:3" ht="75" x14ac:dyDescent="0.2">
       <c r="B25" s="24" t="s">
         <v>76</v>
       </c>
@@ -1096,31 +1096,31 @@
         <v>77</v>
       </c>
     </row>
-    <row r="26" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B26" s="29" t="s">
+    <row r="26" spans="2:3" ht="15" x14ac:dyDescent="0.2">
+      <c r="B26" s="34" t="s">
         <v>12</v>
       </c>
       <c r="C26" s="15" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="27" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B27" s="35"/>
+    <row r="27" spans="2:3" ht="15" x14ac:dyDescent="0.2">
+      <c r="B27" s="40"/>
       <c r="C27" s="2" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="28" spans="2:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B28" s="30"/>
+    <row r="28" spans="2:3" ht="15" x14ac:dyDescent="0.2">
+      <c r="B28" s="35"/>
       <c r="C28" s="15" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="29" spans="2:3" s="39" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B29" s="37"/>
-      <c r="C29" s="38"/>
-    </row>
-    <row r="30" spans="2:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:3" s="28" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B29" s="26"/>
+      <c r="C29" s="27"/>
+    </row>
+    <row r="30" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B30" s="23" t="s">
         <v>0</v>
       </c>
@@ -1128,7 +1128,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="31" spans="2:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B31" s="14" t="s">
         <v>2</v>
       </c>
@@ -1136,7 +1136,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="32" spans="2:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B32" s="23" t="s">
         <v>64</v>
       </c>
@@ -1144,7 +1144,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="33" spans="2:3" ht="30" x14ac:dyDescent="0.2">
+    <row r="33" spans="2:3" ht="45" x14ac:dyDescent="0.2">
       <c r="B33" s="14" t="s">
         <v>3</v>
       </c>
@@ -1152,7 +1152,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="34" spans="2:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B34" s="23" t="s">
         <v>4</v>
       </c>
@@ -1160,7 +1160,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="35" spans="2:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="2:3" ht="30" x14ac:dyDescent="0.2">
       <c r="B35" s="14" t="s">
         <v>6</v>
       </c>
@@ -1168,13 +1168,13 @@
         <v>18</v>
       </c>
     </row>
-    <row r="36" spans="2:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B36" s="23" t="s">
         <v>8</v>
       </c>
       <c r="C36" s="2"/>
     </row>
-    <row r="37" spans="2:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B37" s="14" t="s">
         <v>9</v>
       </c>
@@ -1182,7 +1182,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="38" spans="2:3" ht="60" x14ac:dyDescent="0.2">
+    <row r="38" spans="2:3" ht="90" x14ac:dyDescent="0.2">
       <c r="B38" s="24" t="s">
         <v>79</v>
       </c>
@@ -1190,22 +1190,22 @@
         <v>77</v>
       </c>
     </row>
-    <row r="39" spans="2:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B39" s="29" t="s">
+    <row r="39" spans="2:3" ht="15" x14ac:dyDescent="0.2">
+      <c r="B39" s="34" t="s">
         <v>12</v>
       </c>
       <c r="C39" s="15" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="40" spans="2:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B40" s="35"/>
+    <row r="40" spans="2:3" ht="15" x14ac:dyDescent="0.2">
+      <c r="B40" s="40"/>
       <c r="C40" s="2" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="41" spans="2:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B41" s="30"/>
+    <row r="41" spans="2:3" ht="15" x14ac:dyDescent="0.2">
+      <c r="B41" s="35"/>
       <c r="C41" s="15" t="s">
         <v>72</v>
       </c>
@@ -1235,7 +1235,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="46" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="46" spans="2:3" ht="30" x14ac:dyDescent="0.2">
       <c r="B46" s="14" t="s">
         <v>3</v>
       </c>
@@ -1271,7 +1271,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="51" spans="2:3" ht="45" x14ac:dyDescent="0.2">
+    <row r="51" spans="2:3" ht="60" x14ac:dyDescent="0.2">
       <c r="B51" s="24" t="s">
         <v>67</v>
       </c>
@@ -1279,16 +1279,16 @@
         <v>69</v>
       </c>
     </row>
-    <row r="52" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B52" s="29" t="s">
+    <row r="52" spans="2:3" ht="15" x14ac:dyDescent="0.2">
+      <c r="B52" s="34" t="s">
         <v>12</v>
       </c>
       <c r="C52" s="15" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="53" spans="2:3" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B53" s="36"/>
+    <row r="53" spans="2:3" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B53" s="41"/>
       <c r="C53" s="3" t="s">
         <v>71</v>
       </c>
@@ -1318,7 +1318,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="58" spans="2:3" ht="30" x14ac:dyDescent="0.2">
+    <row r="58" spans="2:3" ht="45" x14ac:dyDescent="0.2">
       <c r="B58" s="14" t="s">
         <v>3</v>
       </c>
@@ -1356,7 +1356,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="63" spans="2:3" ht="30" x14ac:dyDescent="0.2">
+    <row r="63" spans="2:3" ht="45" x14ac:dyDescent="0.2">
       <c r="B63" s="25" t="s">
         <v>73</v>
       </c>
@@ -1364,22 +1364,22 @@
         <v>24</v>
       </c>
     </row>
-    <row r="64" spans="2:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B64" s="26" t="s">
+    <row r="64" spans="2:3" ht="15" x14ac:dyDescent="0.2">
+      <c r="B64" s="31" t="s">
         <v>12</v>
       </c>
       <c r="C64" s="2" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="65" spans="2:3" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B65" s="27"/>
+    <row r="65" spans="2:3" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B65" s="32"/>
       <c r="C65" s="3" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="66" spans="2:3" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B66" s="28"/>
+    <row r="66" spans="2:3" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B66" s="33"/>
       <c r="C66" s="3" t="s">
         <v>74</v>
       </c>
@@ -1409,7 +1409,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="71" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="71" spans="2:3" ht="30" x14ac:dyDescent="0.2">
       <c r="B71" s="14" t="s">
         <v>3</v>
       </c>
@@ -1445,7 +1445,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="76" spans="2:3" ht="45" x14ac:dyDescent="0.2">
+    <row r="76" spans="2:3" ht="60" x14ac:dyDescent="0.2">
       <c r="B76" s="25" t="s">
         <v>78</v>
       </c>
@@ -1453,29 +1453,29 @@
         <v>77</v>
       </c>
     </row>
-    <row r="77" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B77" s="26" t="s">
+    <row r="77" spans="2:3" ht="15" x14ac:dyDescent="0.2">
+      <c r="B77" s="31" t="s">
         <v>12</v>
       </c>
       <c r="C77" s="2" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="78" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B78" s="27"/>
+    <row r="78" spans="2:3" ht="15" x14ac:dyDescent="0.2">
+      <c r="B78" s="32"/>
       <c r="C78" s="15" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="79" spans="2:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B79" s="28"/>
+    <row r="79" spans="2:3" ht="30" x14ac:dyDescent="0.2">
+      <c r="B79" s="33"/>
       <c r="C79" s="15" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="80" spans="2:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B80" s="31"/>
-      <c r="C80" s="31"/>
+      <c r="B80" s="36"/>
+      <c r="C80" s="36"/>
     </row>
     <row r="81" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B81" s="7" t="s">
@@ -1501,7 +1501,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="84" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="84" spans="2:3" ht="30" x14ac:dyDescent="0.2">
       <c r="B84" s="14" t="s">
         <v>3</v>
       </c>
@@ -1509,7 +1509,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="85" spans="2:3" ht="30" x14ac:dyDescent="0.2">
+    <row r="85" spans="2:3" ht="45" x14ac:dyDescent="0.2">
       <c r="B85" s="8" t="s">
         <v>4</v>
       </c>
@@ -1517,7 +1517,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="86" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="86" spans="2:3" ht="30" x14ac:dyDescent="0.2">
       <c r="B86" s="14" t="s">
         <v>6</v>
       </c>
@@ -1539,7 +1539,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="89" spans="2:3" ht="120" x14ac:dyDescent="0.2">
+    <row r="89" spans="2:3" ht="135" x14ac:dyDescent="0.2">
       <c r="B89" s="25" t="s">
         <v>80</v>
       </c>
@@ -1547,8 +1547,8 @@
         <v>81</v>
       </c>
     </row>
-    <row r="90" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B90" s="26" t="s">
+    <row r="90" spans="2:3" ht="30" x14ac:dyDescent="0.2">
+      <c r="B90" s="31" t="s">
         <v>12</v>
       </c>
       <c r="C90" s="2" t="s">
@@ -1556,13 +1556,13 @@
       </c>
     </row>
     <row r="91" spans="2:3" ht="30" x14ac:dyDescent="0.2">
-      <c r="B91" s="27"/>
+      <c r="B91" s="32"/>
       <c r="C91" s="15" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="92" spans="2:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B92" s="28"/>
+    <row r="92" spans="2:3" ht="30" x14ac:dyDescent="0.2">
+      <c r="B92" s="33"/>
       <c r="C92" s="15" t="s">
         <v>34</v>
       </c>
@@ -1592,7 +1592,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="97" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="97" spans="2:3" ht="30" x14ac:dyDescent="0.2">
       <c r="B97" s="14" t="s">
         <v>3</v>
       </c>
@@ -1630,7 +1630,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="102" spans="2:3" ht="45" x14ac:dyDescent="0.2">
+    <row r="102" spans="2:3" ht="60" x14ac:dyDescent="0.2">
       <c r="B102" s="25" t="s">
         <v>82</v>
       </c>
@@ -1638,7 +1638,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="103" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="103" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B103" s="8" t="s">
         <v>12</v>
       </c>
@@ -1670,7 +1670,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="108" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="108" spans="2:3" ht="30" x14ac:dyDescent="0.2">
       <c r="B108" s="14" t="s">
         <v>3</v>
       </c>
@@ -1708,15 +1708,15 @@
         <v>68</v>
       </c>
     </row>
-    <row r="113" spans="2:3" ht="33" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B113" s="40" t="s">
+    <row r="113" spans="2:3" ht="45" x14ac:dyDescent="0.2">
+      <c r="B113" s="29" t="s">
         <v>85</v>
       </c>
-      <c r="C113" s="41" t="s">
+      <c r="C113" s="30" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="114" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="114" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B114" s="14" t="s">
         <v>12</v>
       </c>
@@ -1748,7 +1748,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="119" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="119" spans="2:3" ht="30" x14ac:dyDescent="0.2">
       <c r="B119" s="14" t="s">
         <v>3</v>
       </c>
@@ -1784,7 +1784,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="124" spans="2:3" ht="120" x14ac:dyDescent="0.2">
+    <row r="124" spans="2:3" ht="135" x14ac:dyDescent="0.2">
       <c r="B124" s="25" t="s">
         <v>86</v>
       </c>
@@ -1792,16 +1792,16 @@
         <v>87</v>
       </c>
     </row>
-    <row r="125" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B125" s="29" t="s">
+    <row r="125" spans="2:3" ht="15" x14ac:dyDescent="0.2">
+      <c r="B125" s="34" t="s">
         <v>12</v>
       </c>
       <c r="C125" s="15" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="126" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B126" s="30"/>
+    <row r="126" spans="2:3" ht="15" x14ac:dyDescent="0.2">
+      <c r="B126" s="35"/>
       <c r="C126" s="2" t="s">
         <v>41</v>
       </c>
@@ -1830,7 +1830,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="131" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="131" spans="2:3" ht="30" x14ac:dyDescent="0.2">
       <c r="B131" s="14" t="s">
         <v>3</v>
       </c>
@@ -1874,7 +1874,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="137" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="137" spans="2:3" ht="30" x14ac:dyDescent="0.2">
       <c r="B137" s="14" t="s">
         <v>45</v>
       </c>
@@ -1882,7 +1882,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="138" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="138" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B138" s="8" t="s">
         <v>12</v>
       </c>

</xml_diff>

<commit_message>
fotos das telas na documentação (in process)
</commit_message>
<xml_diff>
--- a/TCC/APS/CasosUso/CasoUsoGeral.xlsx
+++ b/TCC/APS/CasosUso/CasoUsoGeral.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26327"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\userlocal\Desktop\Etec\TCC\APS\CasosUso\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\erics\Documents\GitHub\tccETEC\Etec\TCC\APS\CasosUso\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D49D46B-1527-4BA1-8434-651B69A2BB2C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720"/>
+    <workbookView xWindow="-19320" yWindow="2595" windowWidth="19440" windowHeight="10590" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -303,7 +304,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -346,7 +347,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="12">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -458,21 +459,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="medium">
         <color indexed="64"/>
       </left>
@@ -491,19 +477,6 @@
         <color indexed="64"/>
       </right>
       <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
       <bottom style="medium">
         <color indexed="64"/>
       </bottom>
@@ -513,34 +486,28 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -557,7 +524,7 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -572,63 +539,72 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -909,984 +885,988 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:C138"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A138" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4:C138"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A105" sqref="A105:XFD105"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="6"/>
-    <col min="2" max="2" width="31.140625" style="9" customWidth="1"/>
-    <col min="3" max="3" width="61.85546875" style="6" customWidth="1"/>
-    <col min="4" max="16384" width="9.140625" style="6"/>
+    <col min="1" max="1" width="9.109375" style="5"/>
+    <col min="2" max="2" width="31.109375" style="8" customWidth="1"/>
+    <col min="3" max="3" width="61.88671875" style="5" customWidth="1"/>
+    <col min="4" max="16384" width="9.109375" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:3" ht="15" x14ac:dyDescent="0.2">
-      <c r="B1" s="37"/>
-      <c r="C1" s="37"/>
-    </row>
-    <row r="2" spans="2:3" ht="15" x14ac:dyDescent="0.2">
-      <c r="B2" s="37"/>
-      <c r="C2" s="37"/>
-    </row>
-    <row r="3" spans="2:3" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="37"/>
-      <c r="C3" s="37"/>
-    </row>
-    <row r="4" spans="2:3" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="11" t="s">
+    <row r="1" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B1" s="31"/>
+      <c r="C1" s="31"/>
+    </row>
+    <row r="2" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B2" s="31"/>
+      <c r="C2" s="31"/>
+    </row>
+    <row r="3" spans="2:3" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B3" s="31"/>
+      <c r="C3" s="31"/>
+    </row>
+    <row r="4" spans="2:3" s="11" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="12" t="s">
+      <c r="C4" s="10" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B5" s="8" t="s">
+    <row r="5" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B5" s="7" t="s">
         <v>2</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="6" spans="2:3" s="13" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="14" t="s">
+    <row r="6" spans="2:3" s="11" customFormat="1" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B6" s="12" t="s">
         <v>65</v>
       </c>
-      <c r="C6" s="15" t="s">
+      <c r="C6" s="13" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="2:3" s="13" customFormat="1" ht="30.75" x14ac:dyDescent="0.25">
-      <c r="B7" s="11" t="s">
+    <row r="7" spans="2:3" s="11" customFormat="1" ht="30.6" x14ac:dyDescent="0.3">
+      <c r="B7" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="C7" s="16" t="s">
+      <c r="C7" s="14" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="8" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B8" s="8" t="s">
+    <row r="8" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B8" s="7" t="s">
         <v>4</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="2:3" s="13" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="14" t="s">
+    <row r="9" spans="2:3" s="11" customFormat="1" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B9" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="15" t="s">
+      <c r="C9" s="13" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="2:3" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="11" t="s">
+    <row r="10" spans="2:3" s="11" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B10" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="C10" s="12"/>
-    </row>
-    <row r="11" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B11" s="8" t="s">
+      <c r="C10" s="10"/>
+    </row>
+    <row r="11" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B11" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="C11" s="17" t="s">
+      <c r="C11" s="15" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="12" spans="2:3" s="13" customFormat="1" ht="45" x14ac:dyDescent="0.2">
-      <c r="B12" s="25" t="s">
+    <row r="12" spans="2:3" s="11" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="B12" s="21" t="s">
         <v>10</v>
       </c>
-      <c r="C12" s="15" t="s">
+      <c r="C12" s="13" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="2:3" ht="15" x14ac:dyDescent="0.2">
-      <c r="B13" s="38" t="s">
+    <row r="13" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B13" s="32" t="s">
         <v>12</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="14" spans="2:3" ht="15" x14ac:dyDescent="0.2">
-      <c r="B14" s="38"/>
+    <row r="14" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B14" s="32"/>
       <c r="C14" s="2" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="15" spans="2:3" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="39"/>
+    <row r="15" spans="2:3" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B15" s="33"/>
       <c r="C15" s="3" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B17" s="8" t="s">
+    <row r="16" spans="2:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="17" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B17" s="42" t="s">
         <v>0</v>
       </c>
-      <c r="C17" s="17" t="s">
+      <c r="C17" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B18" s="14" t="s">
+    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B18" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="C18" s="15" t="s">
+      <c r="C18" s="13" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="19" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B19" s="8" t="s">
+    <row r="19" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B19" s="7" t="s">
         <v>64</v>
       </c>
       <c r="C19" s="2" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="20" spans="2:3" ht="45" x14ac:dyDescent="0.2">
-      <c r="B20" s="14" t="s">
+    <row r="20" spans="2:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="B20" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="C20" s="15" t="s">
+      <c r="C20" s="13" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="21" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B21" s="8" t="s">
+    <row r="21" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B21" s="7" t="s">
         <v>4</v>
       </c>
       <c r="C21" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="22" spans="2:3" ht="30" x14ac:dyDescent="0.2">
-      <c r="B22" s="14" t="s">
+    <row r="22" spans="2:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="B22" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="C22" s="15" t="s">
+      <c r="C22" s="13" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="23" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B23" s="8" t="s">
+    <row r="23" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B23" s="7" t="s">
         <v>8</v>
       </c>
       <c r="C23" s="2"/>
     </row>
-    <row r="24" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B24" s="14" t="s">
+    <row r="24" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B24" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="C24" s="18" t="s">
+      <c r="C24" s="16" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="25" spans="2:3" ht="75" x14ac:dyDescent="0.2">
-      <c r="B25" s="24" t="s">
+    <row r="25" spans="2:3" ht="75" x14ac:dyDescent="0.25">
+      <c r="B25" s="20" t="s">
         <v>76</v>
       </c>
       <c r="C25" s="4" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="26" spans="2:3" ht="15" x14ac:dyDescent="0.2">
-      <c r="B26" s="34" t="s">
+    <row r="26" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B26" s="30" t="s">
         <v>12</v>
       </c>
-      <c r="C26" s="15" t="s">
+      <c r="C26" s="13" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="27" spans="2:3" ht="15" x14ac:dyDescent="0.2">
-      <c r="B27" s="40"/>
+    <row r="27" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B27" s="34"/>
       <c r="C27" s="2" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="28" spans="2:3" ht="15" x14ac:dyDescent="0.2">
+    <row r="28" spans="2:3" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B28" s="35"/>
-      <c r="C28" s="15" t="s">
+      <c r="C28" s="41" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="29" spans="2:3" s="28" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B29" s="26"/>
-      <c r="C29" s="27"/>
-    </row>
-    <row r="30" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B30" s="23" t="s">
+    <row r="29" spans="2:3" s="24" customFormat="1" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B29" s="22"/>
+      <c r="C29" s="23"/>
+    </row>
+    <row r="30" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B30" s="42" t="s">
         <v>0</v>
       </c>
-      <c r="C30" s="17" t="s">
+      <c r="C30" s="1" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="31" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B31" s="14" t="s">
+    <row r="31" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B31" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="C31" s="15" t="s">
+      <c r="C31" s="13" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="32" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B32" s="23" t="s">
+    <row r="32" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B32" s="7" t="s">
         <v>64</v>
       </c>
       <c r="C32" s="2" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="33" spans="2:3" ht="45" x14ac:dyDescent="0.2">
-      <c r="B33" s="14" t="s">
+    <row r="33" spans="2:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="B33" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="C33" s="15" t="s">
+      <c r="C33" s="13" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="34" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B34" s="23" t="s">
+    <row r="34" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B34" s="7" t="s">
         <v>4</v>
       </c>
       <c r="C34" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="35" spans="2:3" ht="30" x14ac:dyDescent="0.2">
-      <c r="B35" s="14" t="s">
+    <row r="35" spans="2:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="B35" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="C35" s="15" t="s">
+      <c r="C35" s="13" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="36" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B36" s="23" t="s">
+    <row r="36" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B36" s="7" t="s">
         <v>8</v>
       </c>
       <c r="C36" s="2"/>
     </row>
-    <row r="37" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B37" s="14" t="s">
+    <row r="37" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B37" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="C37" s="18" t="s">
+      <c r="C37" s="16" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="38" spans="2:3" ht="90" x14ac:dyDescent="0.2">
-      <c r="B38" s="24" t="s">
+    <row r="38" spans="2:3" ht="90" x14ac:dyDescent="0.25">
+      <c r="B38" s="20" t="s">
         <v>79</v>
       </c>
       <c r="C38" s="4" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="39" spans="2:3" ht="15" x14ac:dyDescent="0.2">
-      <c r="B39" s="34" t="s">
+    <row r="39" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B39" s="30" t="s">
         <v>12</v>
       </c>
-      <c r="C39" s="15" t="s">
+      <c r="C39" s="13" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="40" spans="2:3" ht="15" x14ac:dyDescent="0.2">
-      <c r="B40" s="40"/>
+    <row r="40" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B40" s="34"/>
       <c r="C40" s="2" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="41" spans="2:3" ht="15" x14ac:dyDescent="0.2">
+    <row r="41" spans="2:3" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B41" s="35"/>
-      <c r="C41" s="15" t="s">
+      <c r="C41" s="41" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="42" spans="2:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="43" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B43" s="7" t="s">
+    <row r="42" spans="2:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="43" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B43" s="6" t="s">
         <v>0</v>
       </c>
       <c r="C43" s="1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="44" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B44" s="14" t="s">
+    <row r="44" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B44" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="C44" s="15" t="s">
+      <c r="C44" s="13" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="45" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B45" s="23" t="s">
+    <row r="45" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B45" s="7" t="s">
         <v>64</v>
       </c>
       <c r="C45" s="2" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="46" spans="2:3" ht="30" x14ac:dyDescent="0.2">
-      <c r="B46" s="14" t="s">
+    <row r="46" spans="2:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="B46" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="C46" s="15" t="s">
+      <c r="C46" s="13" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="47" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B47" s="23" t="s">
+    <row r="47" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B47" s="7" t="s">
         <v>4</v>
       </c>
       <c r="C47" s="2" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="48" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B48" s="14" t="s">
+    <row r="48" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B48" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="C48" s="15"/>
-    </row>
-    <row r="49" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B49" s="23" t="s">
+      <c r="C48" s="13"/>
+    </row>
+    <row r="49" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B49" s="7" t="s">
         <v>8</v>
       </c>
       <c r="C49" s="2"/>
     </row>
-    <row r="50" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B50" s="14" t="s">
+    <row r="50" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B50" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="C50" s="20" t="s">
+      <c r="C50" s="18" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="51" spans="2:3" ht="60" x14ac:dyDescent="0.2">
-      <c r="B51" s="24" t="s">
+    <row r="51" spans="2:3" ht="60" x14ac:dyDescent="0.25">
+      <c r="B51" s="20" t="s">
         <v>67</v>
       </c>
       <c r="C51" s="4" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="52" spans="2:3" ht="15" x14ac:dyDescent="0.2">
-      <c r="B52" s="34" t="s">
+    <row r="52" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B52" s="30" t="s">
         <v>12</v>
       </c>
-      <c r="C52" s="15" t="s">
+      <c r="C52" s="13" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="53" spans="2:3" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B53" s="41"/>
+    <row r="53" spans="2:3" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B53" s="35"/>
       <c r="C53" s="3" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="54" spans="2:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="55" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B55" s="7" t="s">
+    <row r="54" spans="2:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="55" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B55" s="6" t="s">
         <v>0</v>
       </c>
       <c r="C55" s="1" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="56" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B56" s="14" t="s">
+    <row r="56" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B56" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="C56" s="15" t="s">
+      <c r="C56" s="13" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="57" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B57" s="8" t="s">
+    <row r="57" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B57" s="7" t="s">
         <v>64</v>
       </c>
       <c r="C57" s="2" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="58" spans="2:3" ht="45" x14ac:dyDescent="0.2">
-      <c r="B58" s="14" t="s">
+    <row r="58" spans="2:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="B58" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="C58" s="15" t="s">
+      <c r="C58" s="13" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="59" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B59" s="8" t="s">
+    <row r="59" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B59" s="7" t="s">
         <v>4</v>
       </c>
       <c r="C59" s="2" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="60" spans="2:3" ht="30" x14ac:dyDescent="0.2">
-      <c r="B60" s="14" t="s">
+    <row r="60" spans="2:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="B60" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="C60" s="19" t="s">
+      <c r="C60" s="17" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="61" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B61" s="8" t="s">
+    <row r="61" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B61" s="7" t="s">
         <v>8</v>
       </c>
       <c r="C61" s="2"/>
     </row>
-    <row r="62" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B62" s="14" t="s">
+    <row r="62" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B62" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="C62" s="18" t="s">
+      <c r="C62" s="16" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="63" spans="2:3" ht="45" x14ac:dyDescent="0.2">
-      <c r="B63" s="25" t="s">
+    <row r="63" spans="2:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="B63" s="21" t="s">
         <v>73</v>
       </c>
-      <c r="C63" s="21" t="s">
+      <c r="C63" s="19" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="64" spans="2:3" ht="15" x14ac:dyDescent="0.2">
-      <c r="B64" s="31" t="s">
+    <row r="64" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B64" s="28" t="s">
         <v>12</v>
       </c>
       <c r="C64" s="2" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="65" spans="2:3" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B65" s="32"/>
+    <row r="65" spans="2:3" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B65" s="29"/>
       <c r="C65" s="3" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="66" spans="2:3" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B66" s="33"/>
+    <row r="66" spans="2:3" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B66" s="40"/>
       <c r="C66" s="3" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="67" spans="2:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="68" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B68" s="7" t="s">
+    <row r="67" spans="2:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="68" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B68" s="6" t="s">
         <v>0</v>
       </c>
       <c r="C68" s="1" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="69" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B69" s="14" t="s">
+    <row r="69" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B69" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="C69" s="15" t="s">
+      <c r="C69" s="13" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="70" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B70" s="8" t="s">
+    <row r="70" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B70" s="7" t="s">
         <v>64</v>
       </c>
       <c r="C70" s="2" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="71" spans="2:3" ht="30" x14ac:dyDescent="0.2">
-      <c r="B71" s="14" t="s">
+    <row r="71" spans="2:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="B71" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="C71" s="15" t="s">
+      <c r="C71" s="13" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="72" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B72" s="8" t="s">
+    <row r="72" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B72" s="7" t="s">
         <v>4</v>
       </c>
       <c r="C72" s="2" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="73" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B73" s="14" t="s">
+    <row r="73" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B73" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="C73" s="15"/>
-    </row>
-    <row r="74" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B74" s="8" t="s">
+      <c r="C73" s="13"/>
+    </row>
+    <row r="74" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B74" s="7" t="s">
         <v>8</v>
       </c>
       <c r="C74" s="2"/>
     </row>
-    <row r="75" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B75" s="14" t="s">
+    <row r="75" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B75" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="C75" s="18" t="s">
+      <c r="C75" s="16" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="76" spans="2:3" ht="60" x14ac:dyDescent="0.2">
-      <c r="B76" s="25" t="s">
+    <row r="76" spans="2:3" ht="60" x14ac:dyDescent="0.25">
+      <c r="B76" s="21" t="s">
         <v>78</v>
       </c>
-      <c r="C76" s="19" t="s">
+      <c r="C76" s="17" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="77" spans="2:3" ht="15" x14ac:dyDescent="0.2">
-      <c r="B77" s="31" t="s">
+    <row r="77" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B77" s="28" t="s">
         <v>12</v>
       </c>
       <c r="C77" s="2" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="78" spans="2:3" ht="15" x14ac:dyDescent="0.2">
-      <c r="B78" s="32"/>
-      <c r="C78" s="15" t="s">
+    <row r="78" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B78" s="29"/>
+      <c r="C78" s="13" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="79" spans="2:3" ht="30" x14ac:dyDescent="0.2">
-      <c r="B79" s="33"/>
-      <c r="C79" s="15" t="s">
+    <row r="79" spans="2:3" ht="30.6" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B79" s="40"/>
+      <c r="C79" s="41" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="80" spans="2:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B80" s="36"/>
-      <c r="C80" s="36"/>
-    </row>
-    <row r="81" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B81" s="7" t="s">
+    <row r="80" spans="2:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B80" s="31"/>
+      <c r="C80" s="31"/>
+    </row>
+    <row r="81" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B81" s="6" t="s">
         <v>0</v>
       </c>
       <c r="C81" s="1" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="82" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B82" s="14" t="s">
+    <row r="82" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B82" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="C82" s="15" t="s">
+      <c r="C82" s="13" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="83" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B83" s="8" t="s">
+    <row r="83" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B83" s="7" t="s">
         <v>64</v>
       </c>
       <c r="C83" s="2" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="84" spans="2:3" ht="30" x14ac:dyDescent="0.2">
-      <c r="B84" s="14" t="s">
+    <row r="84" spans="2:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="B84" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="C84" s="15" t="s">
+      <c r="C84" s="13" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="85" spans="2:3" ht="45" x14ac:dyDescent="0.2">
-      <c r="B85" s="8" t="s">
+    <row r="85" spans="2:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="B85" s="7" t="s">
         <v>4</v>
       </c>
       <c r="C85" s="2" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="86" spans="2:3" ht="30" x14ac:dyDescent="0.2">
-      <c r="B86" s="14" t="s">
+    <row r="86" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B86" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="C86" s="15" t="s">
+      <c r="C86" s="13" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="87" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B87" s="8" t="s">
+    <row r="87" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B87" s="7" t="s">
         <v>8</v>
       </c>
       <c r="C87" s="2"/>
     </row>
-    <row r="88" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B88" s="14" t="s">
+    <row r="88" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B88" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="C88" s="18" t="s">
+      <c r="C88" s="16" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="89" spans="2:3" ht="135" x14ac:dyDescent="0.2">
-      <c r="B89" s="25" t="s">
+    <row r="89" spans="2:3" ht="120" x14ac:dyDescent="0.25">
+      <c r="B89" s="21" t="s">
         <v>80</v>
       </c>
-      <c r="C89" s="19" t="s">
+      <c r="C89" s="17" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="90" spans="2:3" ht="30" x14ac:dyDescent="0.2">
-      <c r="B90" s="31" t="s">
+    <row r="90" spans="2:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="B90" s="28" t="s">
         <v>12</v>
       </c>
       <c r="C90" s="2" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="91" spans="2:3" ht="30" x14ac:dyDescent="0.2">
-      <c r="B91" s="32"/>
-      <c r="C91" s="15" t="s">
+    <row r="91" spans="2:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="B91" s="29"/>
+      <c r="C91" s="13" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="92" spans="2:3" ht="30" x14ac:dyDescent="0.2">
-      <c r="B92" s="33"/>
-      <c r="C92" s="15" t="s">
+    <row r="92" spans="2:3" ht="30.6" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B92" s="40"/>
+      <c r="C92" s="41" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="93" spans="2:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="94" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B94" s="7" t="s">
+    <row r="93" spans="2:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="94" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B94" s="6" t="s">
         <v>0</v>
       </c>
       <c r="C94" s="1" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="95" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B95" s="14" t="s">
+    <row r="95" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B95" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="C95" s="15" t="s">
+      <c r="C95" s="13" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="96" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B96" s="8" t="s">
+    <row r="96" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B96" s="7" t="s">
         <v>64</v>
       </c>
       <c r="C96" s="2" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="97" spans="2:3" ht="30" x14ac:dyDescent="0.2">
-      <c r="B97" s="14" t="s">
+    <row r="97" spans="2:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="B97" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="C97" s="15" t="s">
+      <c r="C97" s="13" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="98" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B98" s="8" t="s">
+    <row r="98" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B98" s="7" t="s">
         <v>4</v>
       </c>
       <c r="C98" s="2" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="99" spans="2:3" ht="30" x14ac:dyDescent="0.2">
-      <c r="B99" s="14" t="s">
+    <row r="99" spans="2:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="B99" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="C99" s="19" t="s">
+      <c r="C99" s="17" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="100" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B100" s="8" t="s">
+    <row r="100" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B100" s="7" t="s">
         <v>8</v>
       </c>
       <c r="C100" s="2"/>
     </row>
-    <row r="101" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B101" s="14" t="s">
+    <row r="101" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B101" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="C101" s="20" t="s">
+      <c r="C101" s="18" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="102" spans="2:3" ht="60" x14ac:dyDescent="0.2">
-      <c r="B102" s="25" t="s">
+    <row r="102" spans="2:3" ht="60" x14ac:dyDescent="0.25">
+      <c r="B102" s="21" t="s">
         <v>82</v>
       </c>
-      <c r="C102" s="21" t="s">
+      <c r="C102" s="19" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="103" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B103" s="8" t="s">
+    <row r="103" spans="2:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B103" s="27" t="s">
         <v>12</v>
       </c>
-      <c r="C103" s="2" t="s">
+      <c r="C103" s="3" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="105" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B105" s="10" t="s">
+    <row r="104" spans="2:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="105" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B105" s="36" t="s">
         <v>0</v>
       </c>
-      <c r="C105" s="5" t="s">
+      <c r="C105" s="37" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="106" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B106" s="14" t="s">
+    <row r="106" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B106" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="C106" s="15" t="s">
+      <c r="C106" s="13" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="107" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B107" s="8" t="s">
+    <row r="107" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B107" s="7" t="s">
         <v>64</v>
       </c>
       <c r="C107" s="2" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="108" spans="2:3" ht="30" x14ac:dyDescent="0.2">
-      <c r="B108" s="14" t="s">
+    <row r="108" spans="2:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="B108" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="C108" s="15" t="s">
+      <c r="C108" s="13" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="109" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B109" s="8" t="s">
+    <row r="109" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B109" s="7" t="s">
         <v>4</v>
       </c>
       <c r="C109" s="2" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="110" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B110" s="14" t="s">
+    <row r="110" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B110" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="C110" s="15" t="s">
+      <c r="C110" s="13" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="111" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B111" s="8" t="s">
+    <row r="111" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B111" s="7" t="s">
         <v>8</v>
       </c>
       <c r="C111" s="2"/>
     </row>
-    <row r="112" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B112" s="14" t="s">
+    <row r="112" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B112" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="C112" s="18" t="s">
+      <c r="C112" s="16" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="113" spans="2:3" ht="45" x14ac:dyDescent="0.2">
-      <c r="B113" s="29" t="s">
+    <row r="113" spans="2:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="B113" s="25" t="s">
         <v>85</v>
       </c>
-      <c r="C113" s="30" t="s">
+      <c r="C113" s="26" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="114" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B114" s="14" t="s">
+    <row r="114" spans="2:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B114" s="38" t="s">
         <v>12</v>
       </c>
-      <c r="C114" s="22" t="s">
+      <c r="C114" s="39" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="116" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B116" s="10" t="s">
+    <row r="115" spans="2:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="116" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B116" s="36" t="s">
         <v>0</v>
       </c>
-      <c r="C116" s="5" t="s">
+      <c r="C116" s="37" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="117" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B117" s="14" t="s">
+    <row r="117" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B117" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="C117" s="15" t="s">
+      <c r="C117" s="13" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="118" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B118" s="8" t="s">
+    <row r="118" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B118" s="7" t="s">
         <v>64</v>
       </c>
       <c r="C118" s="2" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="119" spans="2:3" ht="30" x14ac:dyDescent="0.2">
-      <c r="B119" s="14" t="s">
+    <row r="119" spans="2:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="B119" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="C119" s="15" t="s">
+      <c r="C119" s="13" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="120" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B120" s="8" t="s">
+    <row r="120" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B120" s="7" t="s">
         <v>4</v>
       </c>
       <c r="C120" s="2" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="121" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B121" s="14" t="s">
+    <row r="121" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B121" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="C121" s="15"/>
-    </row>
-    <row r="122" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B122" s="8" t="s">
+      <c r="C121" s="13"/>
+    </row>
+    <row r="122" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B122" s="7" t="s">
         <v>8</v>
       </c>
       <c r="C122" s="2"/>
     </row>
-    <row r="123" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B123" s="14" t="s">
+    <row r="123" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B123" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="C123" s="18" t="s">
+      <c r="C123" s="16" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="124" spans="2:3" ht="135" x14ac:dyDescent="0.2">
-      <c r="B124" s="25" t="s">
+    <row r="124" spans="2:3" ht="135" x14ac:dyDescent="0.25">
+      <c r="B124" s="21" t="s">
         <v>86</v>
       </c>
-      <c r="C124" s="19" t="s">
+      <c r="C124" s="17" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="125" spans="2:3" ht="15" x14ac:dyDescent="0.2">
-      <c r="B125" s="34" t="s">
+    <row r="125" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B125" s="30" t="s">
         <v>12</v>
       </c>
-      <c r="C125" s="15" t="s">
+      <c r="C125" s="13" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="126" spans="2:3" ht="15" x14ac:dyDescent="0.2">
+    <row r="126" spans="2:3" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B126" s="35"/>
-      <c r="C126" s="2" t="s">
+      <c r="C126" s="3" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="128" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B128" s="10" t="s">
+    <row r="127" spans="2:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="128" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B128" s="36" t="s">
         <v>0</v>
       </c>
-      <c r="C128" s="5" t="s">
+      <c r="C128" s="37" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="129" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B129" s="14" t="s">
+    <row r="129" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B129" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="C129" s="15" t="s">
+      <c r="C129" s="13" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="130" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B130" s="8" t="s">
+    <row r="130" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B130" s="7" t="s">
         <v>64</v>
       </c>
       <c r="C130" s="2" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="131" spans="2:3" ht="30" x14ac:dyDescent="0.2">
-      <c r="B131" s="14" t="s">
+    <row r="131" spans="2:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="B131" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="C131" s="15" t="s">
+      <c r="C131" s="13" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="132" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B132" s="8" t="s">
+    <row r="132" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B132" s="7" t="s">
         <v>4</v>
       </c>
       <c r="C132" s="2" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="133" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B133" s="14" t="s">
+    <row r="133" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B133" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="C133" s="15"/>
-    </row>
-    <row r="134" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B134" s="8" t="s">
+      <c r="C133" s="13"/>
+    </row>
+    <row r="134" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B134" s="7" t="s">
         <v>8</v>
       </c>
       <c r="C134" s="2"/>
     </row>
-    <row r="135" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B135" s="14" t="s">
+    <row r="135" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B135" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="C135" s="18" t="s">
+      <c r="C135" s="16" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="136" spans="2:3" ht="30" x14ac:dyDescent="0.2">
-      <c r="B136" s="24" t="s">
+    <row r="136" spans="2:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="B136" s="20" t="s">
         <v>43</v>
       </c>
       <c r="C136" s="2" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="137" spans="2:3" ht="30" x14ac:dyDescent="0.2">
-      <c r="B137" s="14" t="s">
+    <row r="137" spans="2:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="B137" s="12" t="s">
         <v>45</v>
       </c>
-      <c r="C137" s="15" t="s">
+      <c r="C137" s="13" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="138" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B138" s="8" t="s">
+    <row r="138" spans="2:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B138" s="27" t="s">
         <v>12</v>
       </c>
-      <c r="C138" s="2" t="s">
+      <c r="C138" s="3" t="s">
         <v>47</v>
       </c>
     </row>

</xml_diff>